<commit_message>
a little garden update
</commit_message>
<xml_diff>
--- a/ProjectIoTGarden_ExcelSheet.xlsx
+++ b/ProjectIoTGarden_ExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stude\Documents\GitHub\HHolben.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC227C4-8C26-47A7-AE05-93880512AD75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB395505-B63D-41B0-B93F-DEFAF854AF21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A62D330E-BCF2-48C6-8A48-05B0B9C77103}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Item</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Tentative pin connections plan</t>
   </si>
   <si>
-    <t>UNO RX</t>
-  </si>
-  <si>
     <t>nil</t>
   </si>
   <si>
@@ -139,6 +136,21 @@
   </si>
   <si>
     <t>UNO Ground</t>
+  </si>
+  <si>
+    <t>https://www.tinkercad.com/things/gcMOuioivVi-copy-of-esp8266-01/editel</t>
+  </si>
+  <si>
+    <t>→         →</t>
+  </si>
+  <si>
+    <t>1 K ohm Resistor, 1 K ohm resistor</t>
+  </si>
+  <si>
+    <t>→                →</t>
+  </si>
+  <si>
+    <t>, Ground</t>
   </si>
 </sst>
 </file>
@@ -448,21 +460,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -484,6 +481,21 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -806,16 +818,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D500EB-124E-4AD0-B6C3-6D8BD2B00363}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="107" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="107" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -839,18 +851,18 @@
       <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="25"/>
+      <c r="H4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="14"/>
+      <c r="I4" s="27"/>
       <c r="M4" t="s">
         <v>11</v>
       </c>
@@ -862,7 +874,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C5" s="15"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
@@ -889,7 +901,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="5">
@@ -904,7 +916,7 @@
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7">
@@ -924,21 +936,21 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="18"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C15" s="19"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E16" t="s">
@@ -946,10 +958,10 @@
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E17" t="s">
@@ -957,18 +969,18 @@
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>33</v>
+      <c r="D18" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E19" t="s">
@@ -979,19 +991,19 @@
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="22" t="s">
         <v>27</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -999,48 +1011,62 @@
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="27" t="s">
-        <v>33</v>
+      <c r="D21" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="22" t="s">
         <v>28</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C23" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="27" t="s">
-        <v>23</v>
+      <c r="D23" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1079,9 @@
     <hyperlink ref="K20" r:id="rId1" location=":~:text=From%20the%20datasheet%2C%20we%20find,can%20draw%20maximum%20170mA%20current." display="https://www.instructables.com/id/ESP8266-Pro-Tips/ - :~:text=From%20the%20datasheet%2C%20we%20find,can%20draw%20maximum%20170mA%20current." xr:uid="{3864D3E3-EE5E-4D3C-9074-68B2F3283166}"/>
     <hyperlink ref="K21" r:id="rId2" location=":~:text=The%20board%20can%20operate%20on,is%207%20to%2012%20volts." display=":~:text=The%20board%20can%20operate%20on,is%207%20to%2012%20volts." xr:uid="{23DEC621-9249-4D19-B385-FE00F5922BB4}"/>
     <hyperlink ref="K22" r:id="rId3" xr:uid="{2D4C75E7-9618-4F45-9824-7A197DBA8689}"/>
+    <hyperlink ref="C30" r:id="rId4" xr:uid="{B0F3D3AA-CE3A-46D4-AB4D-B195024FB1B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
can we imbed the garden?
</commit_message>
<xml_diff>
--- a/ProjectIoTGarden_ExcelSheet.xlsx
+++ b/ProjectIoTGarden_ExcelSheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stude\Documents\GitHub\HHolben.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1685AA3-9630-415A-AB6F-C6DF2D83AFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC02577-FA97-4026-8A94-40E712D5D081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A62D330E-BCF2-48C6-8A48-05B0B9C77103}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A62D330E-BCF2-48C6-8A48-05B0B9C77103}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Power" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Item</t>
   </si>
@@ -154,13 +155,55 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=9QZkCQSHnko&amp;t=212s</t>
+  </si>
+  <si>
+    <t>Resistor 1</t>
+  </si>
+  <si>
+    <t>Resistor 2</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>Voltage Input</t>
+  </si>
+  <si>
+    <t>volts</t>
+  </si>
+  <si>
+    <t>Desired Output</t>
+  </si>
+  <si>
+    <t>Volts</t>
+  </si>
+  <si>
+    <t>Vout / Vin</t>
+  </si>
+  <si>
+    <t>1/(R1+R2)</t>
+  </si>
+  <si>
+    <t>R1+R2</t>
+  </si>
+  <si>
+    <t>amps</t>
+  </si>
+  <si>
+    <t>ohms</t>
+  </si>
+  <si>
+    <t>Current At Output</t>
+  </si>
+  <si>
+    <t>9 volt to 3.3 volt voltage divider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +283,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -446,7 +497,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -499,6 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -823,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D500EB-124E-4AD0-B6C3-6D8BD2B00363}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="107" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -1093,4 +1145,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3F7C35-4980-4A47-A05F-D509075B575A}">
+  <dimension ref="D4:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <f>E7/E6</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <f>E10/E8</f>
+        <v>5.5555555555555559E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <f>1/E11</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14">
+        <f>E12-E8</f>
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15">
+        <f>E7/E14</f>
+        <v>0.625</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
projects page background image?
</commit_message>
<xml_diff>
--- a/ProjectIoTGarden_ExcelSheet.xlsx
+++ b/ProjectIoTGarden_ExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stude\Documents\GitHub\HHolben.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC02577-FA97-4026-8A94-40E712D5D081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534E4AA7-7B96-4057-8B19-2068AC6FC12A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A62D330E-BCF2-48C6-8A48-05B0B9C77103}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Item</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>9 volt to 3.3 volt voltage divider</t>
+  </si>
+  <si>
+    <t>9 volt to 5 volt voltage divider</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -535,6 +541,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -550,7 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -906,18 +912,18 @@
       <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="23" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="27"/>
+      <c r="I4" s="28"/>
       <c r="M4" t="s">
         <v>11</v>
       </c>
@@ -1149,23 +1155,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3F7C35-4980-4A47-A05F-D509075B575A}">
-  <dimension ref="D4:F15"/>
+  <dimension ref="D4:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="28" t="s">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D4" s="23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J4" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>44</v>
       </c>
@@ -1175,19 +1185,37 @@
       <c r="F6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>46</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="F7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>42</v>
       </c>
@@ -1197,55 +1225,110 @@
       <c r="F8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>48</v>
       </c>
       <c r="E10">
         <f>E7/E6</f>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10">
+        <f>K7/K6</f>
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>49</v>
       </c>
       <c r="E11">
         <f>E10/E8</f>
+        <v>3.6666666666666667E-2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11">
+        <f>K10/K8</f>
         <v>5.5555555555555559E-2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>50</v>
       </c>
       <c r="E12">
         <f>1/E11</f>
+        <v>27.272727272727273</v>
+      </c>
+      <c r="J12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12">
+        <f>1/K11</f>
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>41</v>
       </c>
       <c r="E14">
         <f>E12-E8</f>
-        <v>8</v>
+        <v>17.272727272727273</v>
       </c>
       <c r="F14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14">
+        <f>K12-K8</f>
+        <v>8</v>
+      </c>
+      <c r="L14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>53</v>
       </c>
       <c r="E15">
         <f>E7/E14</f>
+        <v>0.19105263157894736</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15">
+        <f>K7/K14</f>
         <v>0.625</v>
       </c>
-      <c r="F15" t="s">
+      <c r="L15" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on a draft for a milligan robotics website
</commit_message>
<xml_diff>
--- a/ProjectIoTGarden_ExcelSheet.xlsx
+++ b/ProjectIoTGarden_ExcelSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stude\Documents\GitHub\HHolben.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534E4AA7-7B96-4057-8B19-2068AC6FC12A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E309C6DC-09A2-4489-A61D-3161B5CABA0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A62D330E-BCF2-48C6-8A48-05B0B9C77103}"/>
   </bookViews>
@@ -21,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>Item</t>
   </si>
@@ -203,6 +197,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>32 volt to 5 volt voltage divider</t>
+  </si>
+  <si>
+    <t>5 volt to 5 volt voltage divider</t>
   </si>
 </sst>
 </file>
@@ -1155,27 +1155,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3F7C35-4980-4A47-A05F-D509075B575A}">
-  <dimension ref="D4:L15"/>
+  <dimension ref="D4:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="52" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D4" s="23" t="s">
         <v>54</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O4" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>44</v>
       </c>
@@ -1194,8 +1202,26 @@
       <c r="L6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6">
+        <v>32</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>46</v>
       </c>
@@ -1214,8 +1240,26 @@
       <c r="L7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>42</v>
       </c>
@@ -1234,13 +1278,37 @@
       <c r="L8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8">
+        <v>1000</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>43</v>
+      </c>
+      <c r="W8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8">
+        <v>100</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="4:25" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>56</v>
+      </c>
+      <c r="X9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>48</v>
       </c>
@@ -1255,8 +1323,22 @@
         <f>K7/K6</f>
         <v>0.55555555555555558</v>
       </c>
-    </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10">
+        <f>P7/P6</f>
+        <v>0.15625</v>
+      </c>
+      <c r="W10" t="s">
+        <v>48</v>
+      </c>
+      <c r="X10">
+        <f>X7/X6</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>49</v>
       </c>
@@ -1271,8 +1353,22 @@
         <f>K10/K8</f>
         <v>5.5555555555555559E-2</v>
       </c>
-    </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11">
+        <f>P10/P8</f>
+        <v>1.5625E-4</v>
+      </c>
+      <c r="W11" t="s">
+        <v>49</v>
+      </c>
+      <c r="X11">
+        <f>X10/X8</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>50</v>
       </c>
@@ -1287,8 +1383,31 @@
         <f>1/K11</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12">
+        <f>1/P11</f>
+        <v>6400</v>
+      </c>
+      <c r="U12">
+        <f>1502</f>
+        <v>1502</v>
+      </c>
+      <c r="W12" t="s">
+        <v>50</v>
+      </c>
+      <c r="X12">
+        <f>1/X11</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="4:25" x14ac:dyDescent="0.3">
+      <c r="U13">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="14" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>41</v>
       </c>
@@ -1309,8 +1428,28 @@
       <c r="L14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14">
+        <f>P12-P8</f>
+        <v>5400</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>52</v>
+      </c>
+      <c r="W14" t="s">
+        <v>41</v>
+      </c>
+      <c r="X14">
+        <f>X12-X8</f>
+        <v>150</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="4:25" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>53</v>
       </c>
@@ -1330,6 +1469,32 @@
       </c>
       <c r="L15" t="s">
         <v>51</v>
+      </c>
+      <c r="O15" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15">
+        <f>P7/P14</f>
+        <v>9.2592592592592596E-4</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>51</v>
+      </c>
+      <c r="W15" t="s">
+        <v>53</v>
+      </c>
+      <c r="X15">
+        <f>X7/X14</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="21:21" x14ac:dyDescent="0.3">
+      <c r="U18">
+        <f>SUM(U12:U16)</f>
+        <v>5402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>